<commit_message>
User Stories - Acceptance Critera
Updated with new User Stories
</commit_message>
<xml_diff>
--- a/Logs/User Stories - Acceptance Criteria.xlsx
+++ b/Logs/User Stories - Acceptance Criteria.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\Y2\S2\Software Engineering\Assignment 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cd549\OneDrive - Canterbury Christ Church University\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41DCA57D-1EEB-484F-8BD7-E3DE52C785C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{41DCA57D-1EEB-484F-8BD7-E3DE52C785C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{793AAAD5-E6B1-4991-9E2A-DD51ADC51153}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{ADFB4776-4ACB-4BCD-AA74-3846904141C1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>User Story</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Link User Database to Program</t>
   </si>
   <si>
-    <t>Link Moduloe/Timetable Database to Program</t>
-  </si>
-  <si>
     <t>Create UI Framework</t>
   </si>
   <si>
@@ -129,7 +126,31 @@
     <t>Hash must not be stored in the same database as the encyrpted password</t>
   </si>
   <si>
-    <t>TODO</t>
+    <t>Test Database - Class Linkages</t>
+  </si>
+  <si>
+    <t>Test Login Feature</t>
+  </si>
+  <si>
+    <t>Must display correct map location</t>
+  </si>
+  <si>
+    <t>Must import information from the database correctly</t>
+  </si>
+  <si>
+    <t>Password must only work with the correct password</t>
+  </si>
+  <si>
+    <t>Link Module/Timetable Database to Program</t>
+  </si>
+  <si>
+    <t>Test Admin Database Editing</t>
+  </si>
+  <si>
+    <t>Admin must be able to edit database and have it update immidiately</t>
+  </si>
+  <si>
+    <t>Must not break exiting functions on update</t>
   </si>
 </sst>
 </file>
@@ -498,17 +519,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BD099FA-7909-44A7-91C6-CDA13C930C17}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="67.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -527,7 +548,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -535,16 +556,16 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -552,13 +573,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -567,7 +588,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -578,7 +599,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -589,7 +610,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -597,10 +618,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -608,10 +629,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -619,10 +640,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -630,23 +651,23 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -654,10 +675,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -665,10 +686,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -676,16 +697,52 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>